<commit_message>
Adição da lista de comandos e atulização de pendencias
</commit_message>
<xml_diff>
--- a/Pendências/03_Planilha com pendências.xlsx
+++ b/Pendências/03_Planilha com pendências.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Pendência</t>
   </si>
@@ -81,13 +82,22 @@
   </si>
   <si>
     <t>Ygor Mattos</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
+  </si>
+  <si>
+    <t>Adicionar form com lista de comandos</t>
+  </si>
+  <si>
+    <t>Sim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +117,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,39 +197,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -523,270 +642,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0743EB-A490-4873-B5DF-F9CCC2C4D072}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" activeCellId="1" sqref="H12:I12 H16:I16"/>
+      <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="H2" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="H3" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="H4" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="H5" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="H6" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="H7" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="H8" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="H9" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="H10" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="H11" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="4">
-        <v>42983</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="H12" s="7">
+        <v>42988</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14">
+        <v>42982</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4">
-        <v>42983</v>
-      </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7">
+        <v>42988</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="6" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="2">
-        <v>42986</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="4">
+        <v>42986</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7">
         <v>42983</v>
       </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="8"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -797,16 +960,67 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
+  <mergeCells count="68">
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
@@ -819,47 +1033,23 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H2:I16">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
+  <conditionalFormatting sqref="J1:K1">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Não"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>